<commit_message>
Add functions to get the length of coloumn/row of a sheet.
</commit_message>
<xml_diff>
--- a/TestTool/test.xlsx
+++ b/TestTool/test.xlsx
@@ -9,15 +9,11 @@
     <sheet name="TestPlan" sheetId="1" r:id="rId4"/>
     <sheet name="TestExecution" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>User Story</t>
   </si>
@@ -119,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -131,7 +127,12 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b/>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -142,14 +143,14 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="15"/>
+      <color indexed="14"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -168,66 +169,29 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -247,22 +211,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
         <color indexed="13"/>
@@ -271,7 +220,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -280,13 +229,43 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
         <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
@@ -295,123 +274,98 @@
         <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="12"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0">
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="5">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="7">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="8">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="10">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="8">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="4"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,9 +383,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffbdd6ee"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffbdd6ee"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
@@ -1501,198 +1454,181 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.8516" customWidth="1" style="1"/>
-    <col min="2" max="2" width="12.5" customWidth="1" style="1"/>
-    <col min="3" max="4" width="16.3516" customWidth="1" style="1"/>
-    <col min="14" max="18" width="16.3516" customWidth="1" style="1"/>
-    <col min="19" max="265" width="16.3516" customWidth="1" style="1"/>
+    <col min="1" max="1" width="18.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
+    <col min="3" max="9" width="16.3516" style="1" customWidth="1"/>
+    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="27" customHeight="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="5"/>
-    </row>
-    <row r="2" ht="27" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="B1" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C1" t="s" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D1" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E1" t="s" s="3">
         <v>4</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="F1" t="s" s="3">
         <v>5</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="G1" t="s" s="3">
         <v>6</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="H1" t="s" s="3">
         <v>7</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="I1" t="s" s="3">
         <v>8</v>
       </c>
-      <c r="R2" s="7" t="s">
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" t="s" s="2">
         <v>9</v>
       </c>
+      <c r="B2" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s" s="3">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s" s="3">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" t="s" s="6">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s" s="6">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" t="s" s="3">
         <v>11</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8"/>
-      <c r="N3" s="7" t="s">
+      <c r="F3" t="s" s="7">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" ht="20.35" customHeight="1">
+      <c r="A4" t="s" s="8">
         <v>12</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="B4" t="s" s="9">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="12">
         <v>12</v>
       </c>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="9"/>
-    </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-      <c r="N4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" t="s" s="13">
         <v>16</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="N5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
+      <c r="E5" t="s" s="15">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s" s="15">
+        <v>11</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="N6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="20"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="20"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="20"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-    </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
   </sheetData>
-  <mergeCells>
-    <mergeCell ref="A1:R1"/>
-  </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -1712,322 +1648,322 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="9" width="16.3516" customWidth="1" style="22"/>
-    <col min="10" max="256" width="16.3516" customWidth="1" style="22"/>
+    <col min="1" max="9" width="16.3516" style="18" customWidth="1"/>
+    <col min="10" max="256" width="16.3516" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" t="s" s="19">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s" s="19">
         <v>18</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="C1" t="s" s="19">
         <v>19</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="D1" t="s" s="19">
         <v>20</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="E1" t="s" s="19">
         <v>21</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" t="s" s="19">
         <v>22</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="G1" t="s" s="19">
         <v>23</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="H1" t="s" s="19">
         <v>24</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="I1" t="s" s="19">
         <v>25</v>
       </c>
-      <c r="I1" s="23" t="s">
+    </row>
+    <row r="2" ht="20.35" customHeight="1">
+      <c r="A2" t="s" s="8">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" s="12" t="s">
+      <c r="B2" t="s" s="9">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" t="s" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s" s="13">
+        <v>4</v>
+      </c>
+      <c r="C3" s="14"/>
+      <c r="D3" t="s" s="15">
+        <v>13</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" ht="20.05" customHeight="1">
+      <c r="A4" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s" s="13">
+        <v>4</v>
+      </c>
+      <c r="C4" s="14"/>
+      <c r="D4" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="20.05" customHeight="1">
+      <c r="A5" t="s" s="12">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s" s="13">
+        <v>4</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" t="s" s="15">
+        <v>16</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" t="s" s="15">
         <v>27</v>
       </c>
-      <c r="B2" s="13" t="s">
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" t="s" s="15">
+        <v>10</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    </row>
+    <row r="7" ht="20.05" customHeight="1">
+      <c r="A7" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="B7" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="C7" s="14"/>
+      <c r="D7" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" ht="20.05" customHeight="1">
+      <c r="A8" t="s" s="12">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19" t="s">
+      <c r="C8" s="14"/>
+      <c r="D8" t="s" s="15">
         <v>16</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="19" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="16" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" t="s" s="15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" ht="20.05" customHeight="1">
+      <c r="A9" t="s" s="12">
         <v>29</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19" t="s">
+      <c r="B9" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" t="s" s="15">
+        <v>16</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" t="s" s="15">
         <v>11</v>
       </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="19" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="20"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="20"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="20"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="20"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
+      <c r="A14" s="16"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="20"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="20"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="20"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="20"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
Create class DataModel to store Revision/Tests as key and dataModel as value in Dictionary.
</commit_message>
<xml_diff>
--- a/TestTool/test.xlsx
+++ b/TestTool/test.xlsx
@@ -9,11 +9,12 @@
     <sheet name="TestPlan" sheetId="1" r:id="rId4"/>
     <sheet name="TestExecution" sheetId="2" r:id="rId5"/>
   </sheets>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>User Story</t>
   </si>
@@ -33,9 +34,6 @@
     <t>Rev2</t>
   </si>
   <si>
-    <t>Defect link</t>
-  </si>
-  <si>
     <t>Deviation/Justfication</t>
   </si>
   <si>
@@ -103,36 +101,24 @@
   </si>
   <si>
     <t>PAN-7</t>
-  </si>
-  <si>
-    <t>Rev3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="d-m-yy h:mm:ss"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -143,7 +129,7 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -186,7 +172,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -299,72 +285,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+  <cellXfs count="22">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="3">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="5">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="6">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="7">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1"/>
+    <xf numFmtId="59" fontId="2" fillId="3" borderId="8">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="2" fillId="3" borderId="4">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1460,116 +1465,100 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="18.8516" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="1" customWidth="1"/>
-    <col min="3" max="9" width="16.3516" style="1" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.8516" customWidth="1" style="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1" style="1"/>
+    <col min="3" max="4" width="16.3516" customWidth="1" style="1"/>
+    <col min="10" max="256" width="16.3516" customWidth="1" style="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27" customHeight="1">
-      <c r="A1" t="s" s="2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="3">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="3">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="3">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="3">
+      <c r="G1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="3">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="3">
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" t="s" s="6">
+      <c r="A3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s" s="6">
-        <v>13</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
-      <c r="E3" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s" s="7">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" t="s" s="8">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s" s="9">
-        <v>15</v>
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
-      <c r="E4" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>11</v>
-      </c>
-      <c r="G4" s="10"/>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="12">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s" s="13">
-        <v>16</v>
+      <c r="A5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
-      <c r="E5" t="s" s="15">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s" s="15">
-        <v>11</v>
-      </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="15" t="s">
+        <v>10</v>
+      </c>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
     </row>
@@ -1578,8 +1567,6 @@
       <c r="B6" s="17"/>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
@@ -1589,8 +1576,6 @@
       <c r="B7" s="17"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
@@ -1600,8 +1585,6 @@
       <c r="B8" s="17"/>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -1611,8 +1594,6 @@
       <c r="B9" s="17"/>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -1622,8 +1603,6 @@
       <c r="B10" s="17"/>
       <c r="C10" s="14"/>
       <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -1648,189 +1627,207 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="9" width="16.3516" style="18" customWidth="1"/>
-    <col min="10" max="256" width="16.3516" style="18" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" customWidth="1" style="18"/>
+    <col min="6" max="6" width="23.1797" customWidth="1" style="18"/>
+    <col min="7" max="9" width="16.3516" customWidth="1" style="18"/>
+    <col min="10" max="256" width="16.3516" customWidth="1" style="18"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
-      <c r="A1" t="s" s="19">
+      <c r="A1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s" s="19">
+      <c r="C1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s" s="19">
+      <c r="D1" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s" s="19">
+      <c r="E1" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s" s="19">
+      <c r="F1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s" s="19">
+      <c r="G1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s" s="19">
+      <c r="H1" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="H1" t="s" s="19">
+      <c r="I1" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s" s="19">
+    </row>
+    <row r="2" ht="20.35" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" ht="20.35" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s" s="9">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="D2" t="s" s="11">
-        <v>10</v>
+      <c r="D2" s="11" t="s">
+        <v>9</v>
       </c>
       <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="F2" s="20">
+        <v>41812.546099537038</v>
+      </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
-      <c r="I2" t="s" s="11">
-        <v>11</v>
+      <c r="I2" s="11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" t="s" s="12">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s" s="13">
+      <c r="A3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="14"/>
-      <c r="D3" t="s" s="15">
-        <v>13</v>
+      <c r="D3" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
+      <c r="F3" s="20">
+        <v>41811.546099537038</v>
+      </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
-      <c r="I3" t="s" s="15">
-        <v>11</v>
+      <c r="I3" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="12">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s" s="13">
+      <c r="A4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="D4" t="s" s="15">
-        <v>15</v>
+      <c r="D4" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
+      <c r="F4" s="20">
+        <v>41810.546099537038</v>
+      </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
-      <c r="I4" t="s" s="15">
-        <v>11</v>
+      <c r="I4" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="12">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s" s="13">
+      <c r="A5" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="14"/>
-      <c r="D5" t="s" s="15">
-        <v>16</v>
+      <c r="D5" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
+      <c r="F5" s="20">
+        <v>41809.546099537038</v>
+      </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
-      <c r="I5" t="s" s="15">
+      <c r="I5" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" ht="20.05" customHeight="1">
+      <c r="A6" s="12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="12">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s" s="13">
+      <c r="B6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" t="s" s="15">
-        <v>10</v>
+      <c r="D6" s="15" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
+      <c r="F6" s="20">
+        <v>41808.546099537038</v>
+      </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
-      <c r="I6" t="s" s="15">
-        <v>11</v>
+      <c r="I6" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="12">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s" s="13">
+      <c r="A7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="14"/>
-      <c r="D7" t="s" s="15">
-        <v>15</v>
+      <c r="D7" s="15" t="s">
+        <v>14</v>
       </c>
       <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="F7" s="20">
+        <v>41807.546099537038</v>
+      </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" t="s" s="15">
-        <v>11</v>
+      <c r="I7" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="12">
-        <v>28</v>
-      </c>
-      <c r="B8" t="s" s="13">
+      <c r="A8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="14"/>
-      <c r="D8" t="s" s="15">
-        <v>16</v>
+      <c r="D8" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
+      <c r="F8" s="20">
+        <v>41806.546099537038</v>
+      </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" t="s" s="15">
-        <v>11</v>
+      <c r="I8" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="12">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s" s="13">
-        <v>30</v>
+      <c r="A9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>4</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" t="s" s="15">
-        <v>16</v>
+      <c r="D9" s="15" t="s">
+        <v>15</v>
       </c>
       <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
+      <c r="F9" s="21">
+        <v>41814.546099537038</v>
+      </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" t="s" s="15">
-        <v>11</v>
+      <c r="I9" s="15" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">

</xml_diff>